<commit_message>
minor fixes in data
</commit_message>
<xml_diff>
--- a/public/public_data/v1.6/EpiGenes_complexes_1_6.xlsx
+++ b/public/public_data/v1.6/EpiGenes_complexes_1_6.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'EpiGenes_complexes_1.5'!$B$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'EpiGenes_complexes_1.5'!$B$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'EpiGenes_complexes_1.5'!$B$1:$Q$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'EpiGenes_complexes_1.5'!$B$1:$Q$70</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -1088,7 +1089,7 @@
     <t>16634648, 17617668</t>
   </si>
   <si>
-    <t>Mediates the ATP-dependent exchange of histone H2AZ/H2B dimers for nucleosomal H2A/H2B, leading to transcriptional regulation of selected genes by chromatin remodeling. "SRCAP-containing complex supports ATP-dependent exchange of histone dimers containing H2B and H2A.Z into mononucleosomes reconstituted with recombinant H2A, H2B, H3, and H4", PMID: 16634648.</t>
+    <t>Mediates the ATP-dependent exchange of histone H2AZ/H2B dimers for nucleosomal H2A/H2B, leading to transcriptional regulation of selected genes by chromatin remodeling. SRCAP-containing complex supports ATP-dependent exchange of histone dimers containing H2B and H2A.Z into mononucleosomes reconstituted with recombinant H2A, H2B, H3, and H4.</t>
   </si>
   <si>
     <t>DUB</t>
@@ -1527,9 +1528,9 @@
   <dimension ref="A1:IX70"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="N60" activeCellId="0" sqref="N60"/>
+      <selection pane="bottomLeft" activeCell="Q60" activeCellId="0" sqref="Q60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>